<commit_message>
[FIX] titulo completo añadido
</commit_message>
<xml_diff>
--- a/datosMozillaBlog.xlsx
+++ b/datosMozillaBlog.xlsx
@@ -418,7 +418,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sin título</v>
+        <v>Improving Firefox Stability in the Enterprise by Reducing DLL Injection</v>
       </c>
       <c r="B2" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2021/10/biophoto-72x72.png</v>
@@ -429,7 +429,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Sin título</v>
+        <v>Launching Interop 2025</v>
       </c>
       <c r="B3" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2020/11/ravengfairy006-72x72.jpg</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Sin título</v>
+        <v>Introducing Uniffi for React Native: Rust-Powered Turbo Modules</v>
       </c>
       <c r="B4" t="str">
         <v>https://secure.gravatar.com/avatar/dcea6b39c498494e270e1352fd9efa38?s=72&amp;d=mm&amp;r=g</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Sin título</v>
+        <v>Llamafile v0.8.14: a new UI, performance gains, and more</v>
       </c>
       <c r="B5" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2024/10/cropped-stephen-hood-headshot-72x72.png</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Sin título</v>
+        <v>0Din: A GenAI Bug Bounty Program – Securing Tomorrow’s AI Together</v>
       </c>
       <c r="B6" t="str">
         <v>https://secure.gravatar.com/avatar/28bd0fd405165ce1f924b262aad30e49?s=72&amp;d=mm&amp;r=g</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Sin título</v>
+        <v>Announcing Official Puppeteer Support for Firefox</v>
       </c>
       <c r="B7" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2020/11/ravengfairy006-72x72.jpg</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Sin título</v>
+        <v>Snapshots for IPC Fuzzing</v>
       </c>
       <c r="B8" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2024/06/cropped-export2-small-square-72x72.jpg</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Sin título</v>
+        <v>Sponsoring sqlite-vec to enable more powerful Local AI applications</v>
       </c>
       <c r="B9" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2024/10/cropped-stephen-hood-headshot-72x72.png</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Sin título</v>
+        <v>Experimenting with local alt text generation in Firefox Nightly</v>
       </c>
       <c r="B10" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2024/05/cropped-250019-72x72.jpg</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Sin título</v>
+        <v>Llamafile’s progress, four months in</v>
       </c>
       <c r="B11" t="str">
         <v>https://hacks.mozilla.org/wp-content/uploads/2024/10/cropped-stephen-hood-headshot-72x72.png</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Sin título</v>
+        <v>Porting a cross-platform GUI application to Rust</v>
       </c>
       <c r="B12" t="str">
         <v>https://secure.gravatar.com/avatar/96d490ad54610a265a7fcc4d0ac2a3b6?s=72&amp;d=mm&amp;r=g</v>

</xml_diff>